<commit_message>
added Fan to hardware list
</commit_message>
<xml_diff>
--- a/Hardware summary.xlsx
+++ b/Hardware summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\gitprojects\PET-to-Filament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847E169B-D355-4822-8584-C653F0FB7573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4854EC13-5651-4684-9E46-732D8D3C274E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5008AEBF-8BF8-4753-B41C-CB0E443F1CDB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Power supply 12V 10A (120W)</t>
   </si>
@@ -158,12 +158,6 @@
 WITH anya</t>
   </si>
   <si>
-    <t>Az L vasat a fához való rögzítésre. Telsejmenetes legyen, ne részmenetes</t>
-  </si>
-  <si>
-    <t>6mm széles, lapvastagság + anyavastagság hosszú csavar; anyával; alátéttel</t>
-  </si>
-  <si>
     <t>M8 Threaded Rod (500mm)
  + 2db anya + 2db alátét</t>
   </si>
@@ -212,6 +206,13 @@
   </si>
   <si>
     <t>Plusz&amp;roll</t>
+  </si>
+  <si>
+    <t>12V fan</t>
+  </si>
+  <si>
+    <t>It is important to cool down the filamen as soon as it gets through the noozle in order to avoid further deformation
+60x60x10mm</t>
   </si>
 </sst>
 </file>
@@ -637,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E5B270-1201-49D6-8559-7B56D2A3F6E6}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,10 +664,10 @@
         <v>18</v>
       </c>
       <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -700,7 +701,7 @@
         <v>3790</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -721,7 +722,7 @@
         <v>8568</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -742,7 +743,7 @@
         <v>1100</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -763,7 +764,7 @@
         <v>3950</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -802,7 +803,7 @@
         <v>957</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -823,7 +824,7 @@
         <v>950</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -881,11 +882,11 @@
         <v>31</v>
       </c>
       <c r="D13" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E13" s="11">
         <f>D13*234</f>
-        <v>234</v>
+        <v>702</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -906,7 +907,7 @@
         <v>480</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I14" t="s">
         <v>32</v>
@@ -932,7 +933,7 @@
     </row>
     <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>27</v>
@@ -950,7 +951,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" s="5">
         <f>11+6+1+4+1</f>
@@ -963,7 +964,7 @@
     </row>
     <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>28</v>
@@ -981,7 +982,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D19">
         <f>26+4+4+2+6+2+4</f>
@@ -994,13 +995,13 @@
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -1010,12 +1011,12 @@
         <v>2310</v>
       </c>
       <c r="G20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>33</v>
@@ -1034,7 +1035,7 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
@@ -1074,32 +1075,38 @@
         <v>520</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B25" s="1"/>
       <c r="C25" s="2"/>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <f>D26*966</f>
+        <v>1932</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D27" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E27" s="3">
         <f>SUM(E2:E23)</f>
-        <v>25258</v>
+        <v>25726</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1131,8 +1138,9 @@
     <hyperlink ref="C11" r:id="rId19" xr:uid="{4873F704-FD1F-448F-816D-648F5206FF88}"/>
     <hyperlink ref="C24" r:id="rId20" xr:uid="{FC8A903A-E6F2-4150-A81B-C4BBA202E710}"/>
     <hyperlink ref="D27" r:id="rId21" xr:uid="{30E68C9B-BA6A-4787-B6BB-86B7D7EA421B}"/>
+    <hyperlink ref="C26" r:id="rId22" xr:uid="{7B7F70EA-B7A4-493D-BA75-D1D657E16464}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added styling for better readability
</commit_message>
<xml_diff>
--- a/Hardware summary.xlsx
+++ b/Hardware summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orgog\gitprojects\PET-to-Filament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718128B8-04F6-4CA1-8178-9EE1E27595C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13638519-CE09-4142-9512-86D965385B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5008AEBF-8BF8-4753-B41C-CB0E443F1CDB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="101">
   <si>
     <t>Power supply 12V 10A (120W)</t>
   </si>
@@ -218,9 +218,6 @@
     <t>HUF</t>
   </si>
   <si>
-    <t>Electricity usage in 60mins</t>
-  </si>
-  <si>
     <t>1000g filament</t>
   </si>
   <si>
@@ -255,9 +252,6 @@
   </si>
   <si>
     <t>IS</t>
-  </si>
-  <si>
-    <t>Please modify the green backgrounded fields with the appropriate data:</t>
   </si>
   <si>
     <t>USD</t>
@@ -326,9 +320,6 @@
     <t>My local conditions</t>
   </si>
   <si>
-    <t>If you add all 3 of these, the summary page will use your numbers instead of mine</t>
-  </si>
-  <si>
     <t>SUM purchased parts</t>
   </si>
   <si>
@@ -354,6 +345,65 @@
   </si>
   <si>
     <t>Motor speedcontroller holder</t>
+  </si>
+  <si>
+    <t>click the text above to see the original list on Petamentor2 website</t>
+  </si>
+  <si>
+    <t>Printer electricity usage in 60mins</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If you add </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all 3 of these</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, the summary page will use your numbers instead of mine</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please modify the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>green backgrounded</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fields with the appropriate data relevant for you:</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -364,7 +414,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +524,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -501,11 +588,304 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="22">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -515,15 +895,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -562,14 +936,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -602,10 +970,134 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -925,138 +1417,154 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C17CE76-1C92-489A-84D7-42020B6C1ACE}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="26"/>
+    </row>
+    <row r="5" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="6" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+    </row>
+    <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+      <c r="A9" s="28"/>
+    </row>
+    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10">
+      <c r="B10" s="33">
         <v>1</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="34" t="str">
         <f>B8</f>
         <v>USD</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10">
+      <c r="D10" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="38">
         <v>380</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="34" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+      <c r="A11" s="28"/>
+    </row>
+    <row r="12" spans="1:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="28"/>
+    </row>
+    <row r="13" spans="1:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="64"/>
+      <c r="B13" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="2" t="str">
+      <c r="C13" s="66" t="str">
         <f>B8</f>
         <v>USD</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="3">
+    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+      <c r="A14" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="60">
         <f>'Parts to buy'!G25</f>
         <v>27941</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="61">
         <f>'Parts to buy'!H25</f>
         <v>73.528947368421058</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="2">
+    <row r="15" spans="1:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="62">
         <f>'Printed parts'!G20</f>
         <v>2728.6538400000004</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="63">
         <f>IF(AND(NOT(ISBLANK('Printed parts'!F4)),NOT(ISBLANK('Printed parts'!F5)),NOT(ISBLANK('Printed parts'!F6))),'Printed parts'!H20,Summary!B15/Summary!E10)</f>
         <v>7.1806680000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+      <c r="A16" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="68">
         <f>SUM(B14:B15)</f>
         <v>30669.653839999999</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="69">
         <f>SUM(C14:C15)</f>
         <v>80.709615368421055</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E5B270-1201-49D6-8559-7B56D2A3F6E6}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="2" max="2" width="34.5546875" customWidth="1"/>
-    <col min="3" max="3" width="67.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.109375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.44140625" customWidth="1"/>
     <col min="6" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
@@ -1065,310 +1573,310 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="28"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="7" t="str">
+      <c r="H1" s="5" t="str">
         <f>_xlfn.CONCAT("price sum [",Summary!B8,"]")</f>
         <v>price sum [USD]</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <f>2600+1190</f>
         <v>3790</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="14">
         <f>Summary!$B$10*'Parts to buy'!G2/Summary!$E$10</f>
         <v>9.973684210526315</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="2">
+      <c r="E3" s="4"/>
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <f>5548+3020</f>
         <v>8568</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="14">
         <f>Summary!$B$10*'Parts to buy'!G3/Summary!$E$10</f>
         <v>22.547368421052632</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="2">
+      <c r="E4" s="4"/>
+      <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <f>1100</f>
         <v>1100</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="14">
         <f>Summary!$B$10*'Parts to buy'!G4/Summary!$E$10</f>
         <v>2.8947368421052633</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="2">
+      <c r="E5" s="4"/>
+      <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <f>3000+950</f>
         <v>3950</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="14">
         <f>Summary!$B$10*'Parts to buy'!G5/Summary!$E$10</f>
         <v>10.394736842105264</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="2">
+      <c r="E6" s="4"/>
+      <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <f>1077+447</f>
         <v>1524</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="14">
         <f>Summary!$B$10*'Parts to buy'!G6/Summary!$E$10</f>
         <v>4.0105263157894733</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="2">
+      <c r="E7" s="4"/>
+      <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <f>460+490</f>
         <v>950</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="14">
         <f>Summary!$B$10*'Parts to buy'!G7/Summary!$E$10</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>2</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <f>F8*100</f>
         <v>200</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="14">
         <f>Summary!$B$10*'Parts to buy'!G8/Summary!$E$10</f>
         <v>0.52631578947368418</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>3</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <f>F9*234</f>
         <v>702</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="14">
         <f>Summary!$B$10*'Parts to buy'!G9/Summary!$E$10</f>
         <v>1.8473684210526315</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>2</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <f>F10*966</f>
         <v>1932</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="14">
         <f>Summary!$B$10*'Parts to buy'!G10/Summary!$E$10</f>
         <v>5.0842105263157897</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="5"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="2">
+      <c r="E12" s="4"/>
+      <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <f>482+475</f>
         <v>957</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="14">
         <f>Summary!$B$10*'Parts to buy'!G12/Summary!$E$10</f>
         <v>2.5184210526315791</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="13" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="2">
+      <c r="E13" s="4"/>
+      <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <f>480</f>
         <v>480</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="14">
         <f>Summary!$B$10*'Parts to buy'!G13/Summary!$E$10</f>
         <v>1.263157894736842</v>
       </c>
@@ -1377,271 +1885,276 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="E15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="1">
         <v>1</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>520</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="14">
         <f>Summary!$B$10*'Parts to buy'!G15/Summary!$E$10</f>
         <v>1.368421052631579</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="E16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="1">
         <v>1</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>100</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="14">
         <f>Summary!$B$10*'Parts to buy'!G16/Summary!$E$10</f>
         <v>0.26315789473684209</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
-      <c r="B17" s="14" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="D17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="1">
         <f>11+6+1+4+1</f>
         <v>23</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <f>F17*9</f>
         <v>207</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="14">
         <f>Summary!$B$10*'Parts to buy'!G17/Summary!$E$10</f>
         <v>0.54473684210526319</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="23"/>
+      <c r="B18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="D18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="1">
         <v>3</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <f>F18*85</f>
         <v>255</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="14">
         <f>Summary!$B$10*'Parts to buy'!G18/Summary!$E$10</f>
         <v>0.67105263157894735</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="23"/>
+      <c r="B19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="D19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="1">
         <v>5</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <f>F19*16</f>
         <v>80</v>
       </c>
-      <c r="H19" s="17">
+      <c r="H19" s="14">
         <f>Summary!$B$10*'Parts to buy'!G19/Summary!$E$10</f>
         <v>0.21052631578947367</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
-      <c r="B20" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="E20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="1">
         <v>1</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>520</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="14">
         <f>Summary!$B$10*'Parts to buy'!G20/Summary!$E$10</f>
         <v>1.368421052631579</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="23"/>
+      <c r="B21" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>2</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <f>(480*F21)+510</f>
         <v>1470</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H21" s="14">
         <f>Summary!$B$10*'Parts to buy'!G21/Summary!$E$10</f>
         <v>3.8684210526315788</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="27"/>
-      <c r="B22" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="A22" s="23"/>
+      <c r="B22" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="E22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="1">
         <f>26+4+4+2+6+2+4</f>
         <v>48</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
         <f>F22*6</f>
         <v>288</v>
       </c>
-      <c r="H22" s="17">
+      <c r="H22" s="14">
         <f>Summary!$B$10*'Parts to buy'!G22/Summary!$E$10</f>
         <v>0.75789473684210529</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="27"/>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="23"/>
+      <c r="B23" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="E23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="1">
         <v>3</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <f>116*F23</f>
         <v>348</v>
       </c>
-      <c r="H23" s="17">
+      <c r="H23" s="14">
         <f>Summary!$B$10*'Parts to buy'!G23/Summary!$E$10</f>
         <v>0.91578947368421049</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="5"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="G25" s="19">
+      <c r="B25" s="1"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="15">
         <f>SUM(G2:G23)</f>
         <v>27941</v>
       </c>
-      <c r="H25" s="20">
+      <c r="H25" s="16">
         <f>SUM(H2:H23)</f>
         <v>73.528947368421058</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F26" s="39" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1682,560 +2195,574 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98662D7E-E6BD-4BF9-AEAE-A6857819FA62}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:9" s="7" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
         <v>65</v>
       </c>
     </row>
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="F3" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="29"/>
+      <c r="A3" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="E3" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="40">
         <v>72</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="G4" t="str">
+      <c r="E4" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="40" t="str">
         <f>Summary!B8</f>
         <v>USD</v>
       </c>
-      <c r="H4" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4" s="30"/>
+      <c r="H4" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="40">
+        <v>0.126</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="41"/>
+      <c r="G5" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B5">
-        <v>0.126</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6">
+      <c r="B6" s="40">
         <v>6262</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="G6" t="str">
+      <c r="E6" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="41"/>
+      <c r="G6" s="40" t="str">
         <f>Summary!B8</f>
         <v>USD</v>
       </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="1" t="str">
+      <c r="F8" s="50" t="str">
         <f>_xlfn.CONCAT("Price/piece [",Summary!B8,"]")</f>
         <v>Price/piece [USD]</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" s="1" t="str">
+      <c r="G8" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="51" t="str">
         <f>_xlfn.CONCAT("Sum price [",Summary!B8,"]")</f>
         <v>Sum price [USD]</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="53">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="43">
         <v>7</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="43">
         <v>0.75</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="44">
         <f t="shared" ref="E9:E19" si="0">((C9*($B$5*$B$4)/60)+((D9*$B$6)/1000))</f>
         <v>5.7549000000000001</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="43">
         <f t="shared" ref="F9:F19" si="1">((C9*($F$5*$F$4)/60)+((D9*$F$6)/1000))</f>
         <v>0</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="44">
         <f t="shared" ref="G9:G19" si="2">((C9*($B$5*$B$4)/60)+((D9*$B$6)/1000))*B9</f>
         <v>34.529400000000003</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="45">
         <f t="shared" ref="H9:H19" si="3">((C9*($F$5*$F$4)/60)+((D9*$F$6)/1000))*B9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="36">
         <v>3</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="37">
         <v>62</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="37">
         <v>13.52</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="42">
         <f t="shared" si="0"/>
         <v>94.036639999999991</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="42">
         <f t="shared" si="2"/>
         <v>282.10991999999999</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="46">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="36">
         <v>1</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="37">
         <f>4*60+10</f>
         <v>250</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="37">
         <v>51.47</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="42">
         <f t="shared" si="0"/>
         <v>360.10514000000001</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="42">
         <f t="shared" si="2"/>
         <v>360.10514000000001</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="46">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="36">
         <v>2</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="37">
         <v>60</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="37">
         <v>14.77</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="42">
         <f t="shared" si="0"/>
         <v>101.56174</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="42">
         <f t="shared" si="2"/>
         <v>203.12348</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="46">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="A13" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="36">
         <v>1</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="37">
         <v>64</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="37">
         <v>8.51</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="42">
         <f t="shared" si="0"/>
         <v>62.966419999999992</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="42">
         <f t="shared" si="2"/>
         <v>62.966419999999992</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="46">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="A14" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="36">
         <v>1</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="37">
         <v>6</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="37">
         <v>0.61</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="42">
         <f t="shared" si="0"/>
         <v>4.7270199999999996</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="42">
         <f t="shared" si="2"/>
         <v>4.7270199999999996</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="46">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="A15" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="36">
         <v>4</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="37">
         <f>(3*60+36)/4</f>
         <v>54</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="37">
         <f>52/4</f>
         <v>13</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="42">
         <f t="shared" si="0"/>
         <v>89.570800000000006</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="42">
         <f t="shared" si="2"/>
         <v>358.28320000000002</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="46">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="36">
         <v>1</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="37">
         <f>7*60+7</f>
         <v>427</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="37">
         <v>92.4</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="42">
         <f t="shared" si="0"/>
         <v>643.17120000000011</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="42">
         <f t="shared" si="2"/>
         <v>643.17120000000011</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="46">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="A17" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="36">
         <v>1</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="37">
         <f>60+25</f>
         <v>85</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="37">
         <v>16.04</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="42">
         <f t="shared" si="0"/>
         <v>113.29447999999999</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="42">
         <f t="shared" si="2"/>
         <v>113.29447999999999</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="46">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" s="2">
+      <c r="A18" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="36">
         <v>1</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="37">
         <f>4*60+24</f>
         <v>264</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="37">
         <v>54.69</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="42">
         <f t="shared" si="0"/>
         <v>382.38558</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="42">
         <f t="shared" si="2"/>
         <v>382.38558</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="46">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="54">
         <v>1</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="47">
         <f>3*60</f>
         <v>180</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="47">
         <v>41</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="48">
         <f t="shared" si="0"/>
         <v>283.95800000000003</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="47">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="48">
         <f t="shared" si="2"/>
         <v>283.95800000000003</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="49">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="F20" s="22" t="s">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="F20" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="19">
         <f>SUM(G9:G19)</f>
         <v>2728.6538400000004</v>
       </c>
-      <c r="H20" s="24">
+      <c r="H20" s="20">
         <f>SUM(H9:H19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:H19">
     <sortCondition ref="A9:A19"/>
   </sortState>
   <mergeCells count="3">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="H4:I6"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>